<commit_message>
plot proportion disease, hosp, death
</commit_message>
<xml_diff>
--- a/_checkllist.xlsx
+++ b/_checkllist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="5280" windowWidth="23840" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="13200" yWindow="9520" windowWidth="23840" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
   <dimension ref="B1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
changes in proba hosp and death fits
</commit_message>
<xml_diff>
--- a/_checkllist.xlsx
+++ b/_checkllist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="880" windowWidth="28540" windowHeight="14360" tabRatio="500"/>
+    <workbookView xWindow="13060" yWindow="1340" windowWidth="28540" windowHeight="14360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,8 @@
     <t xml:space="preserve">interv_efficacy </t>
   </si>
   <si>
-    <t xml:space="preserve">Fit "prob_hosp" adnd "proba_death_mult" on proportions output in "plot_pop.pdf" on desired values ; 
+    <t xml:space="preserve">fit/fit-proba-hosp-death.R
+check "prob_hosp" adnd "proba_death_mult" on proportions output in "plot_pop.pdf" on desired values ; 
 Coarsing issue with small population &amp; low rates </t>
   </si>
 </sst>
@@ -742,7 +743,7 @@
   <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,7 +829,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="56">
+    <row r="6" spans="2:10" ht="84">
       <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
         <v>4</v>

</xml_diff>